<commit_message>
#49 Method index updated to send information to view; Fix error on DataContext with tags DbSet; Migrations; Update apoioMVC.
</commit_message>
<xml_diff>
--- a/documentation/tasks/apoioMVC.xlsx
+++ b/documentation/tasks/apoioMVC.xlsx
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#50 Method on controller created: FrindsSugestion() -> Return to view with sugestions
</commit_message>
<xml_diff>
--- a/documentation/tasks/apoioMVC.xlsx
+++ b/documentation/tasks/apoioMVC.xlsx
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Controller</t>
   </si>
@@ -301,9 +301,6 @@
     <t>FriendsSegestion</t>
   </si>
   <si>
-    <t>Paginas com segestão de amigos</t>
-  </si>
-  <si>
     <t>Mostrar tamanho da sua rede até 3º nivel</t>
   </si>
   <si>
@@ -324,6 +321,23 @@
   </si>
   <si>
     <t>EDITAR</t>
+  </si>
+  <si>
+    <t>Redireciona para o ficheiro executável ~/DownloadGame/game.exe</t>
+  </si>
+  <si>
+    <t>Envia uma lista com todos os 
+amigos não comuns de 
+todos os seu amifgos</t>
+  </si>
+  <si>
+    <t>Paginas com sugestão de amigos</t>
+  </si>
+  <si>
+    <t>PODERÃO SER APRESENTADOS TODOS 
+OU PODE SER CRIADO UM RANDOM 
+(ENTRE 0 E TAMANHO DA LISTA - 1) 
+PARA OS APRESENTAR</t>
   </si>
 </sst>
 </file>
@@ -424,15 +438,9 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -459,6 +467,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,11 +768,11 @@
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="2" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="53.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" customWidth="1"/>
     <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="32.7109375" customWidth="1"/>
@@ -768,545 +782,561 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="J4" s="5" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="J4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
     </row>
     <row r="6" spans="2:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12" t="s">
+      <c r="G6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12" t="s">
+      <c r="E7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
     </row>
     <row r="8" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" ht="105" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12" t="s">
+      <c r="C12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12" t="s">
+      <c r="D13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12" t="s">
+      <c r="D14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="9" t="s">
+      <c r="J14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-    </row>
-    <row r="14" spans="2:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="9" t="s">
+      <c r="L14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#45 Method Search finished. Possible search by name or tags View created but without data show. _NavBarPartial added TextBox to put words to search.
</commit_message>
<xml_diff>
--- a/documentation/tasks/apoioMVC.xlsx
+++ b/documentation/tasks/apoioMVC.xlsx
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Controller</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Gestão de Roles, Semantica de tags, …</t>
   </si>
   <si>
-    <t>Mostrar ScoreBoards do utilizador</t>
-  </si>
-  <si>
     <t>FriendsSugestion</t>
   </si>
   <si>
@@ -271,12 +268,6 @@
   </si>
   <si>
     <t>Visualizar o tamanho da sua rede até 3º Nivel</t>
-  </si>
-  <si>
-    <t>Visualizar a sua tag cloud</t>
-  </si>
-  <si>
-    <t>Visualizar a tag cloud das suas relações</t>
   </si>
   <si>
     <t>_NavBarPartil</t>
@@ -338,6 +329,21 @@
 OU PODE SER CRIADO UM RANDOM 
 (ENTRE 0 E TAMANHO DA LISTA - 1) 
 PARA OS APRESENTAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ViewBag.networkSize</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Efetua pesquisa de utilizadores por nome</t>
+  </si>
+  <si>
+    <t>Mostra o resultado da pesquisa de utilizadores</t>
+  </si>
+  <si>
+    <t>Pesquisa por Nome e Tag</t>
   </si>
 </sst>
 </file>
@@ -756,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +905,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>15</v>
@@ -909,17 +915,23 @@
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -948,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -978,10 +990,10 @@
         <v>19</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -997,27 +1009,33 @@
       <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>27</v>
+      <c r="C10" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -1028,34 +1046,32 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>25</v>
+      <c r="C11" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="G11" s="7"/>
       <c r="H11" s="9"/>
       <c r="I11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
@@ -1068,27 +1084,27 @@
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="9"/>
       <c r="I12" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -1101,27 +1117,21 @@
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="9"/>
       <c r="I13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -1134,30 +1144,24 @@
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="2:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -1176,9 +1180,15 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="I15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
@@ -1325,7 +1335,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -1336,7 +1346,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#51 Add ViewBag in Profile ActionResult to send Network Size 3º level
</commit_message>
<xml_diff>
--- a/documentation/tasks/apoioMVC.xlsx
+++ b/documentation/tasks/apoioMVC.xlsx
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Controller</t>
   </si>
@@ -337,13 +337,13 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Efetua pesquisa de utilizadores por nome</t>
-  </si>
-  <si>
     <t>Mostra o resultado da pesquisa de utilizadores</t>
   </si>
   <si>
     <t>Pesquisa por Nome e Tag</t>
+  </si>
+  <si>
+    <t>Efetua pesquisa de utilizadores por nome e tag</t>
   </si>
 </sst>
 </file>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>30</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>15</v>
@@ -1062,7 +1062,9 @@
       <c r="F11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="10" t="s">
         <v>19</v>
@@ -1091,11 +1093,15 @@
         <v>47</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="9"/>
       <c r="I12" s="10" t="s">
         <v>19</v>
@@ -1187,7 +1193,7 @@
         <v>47</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>

</xml_diff>

<commit_message>
#4 Update on task division
</commit_message>
<xml_diff>
--- a/documentation/tasks/apoioMVC.xlsx
+++ b/documentation/tasks/apoioMVC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Márcio\Dropbox\Faculdade\3º Ano\LAPR5\git\documentation\tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScarePT\Documents\EpicWare\documentation\tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
   <si>
     <t>Controller</t>
   </si>
@@ -331,9 +331,6 @@
 PARA OS APRESENTAR</t>
   </si>
   <si>
-    <t xml:space="preserve"> ViewBag.networkSize</t>
-  </si>
-  <si>
     <t>Search</t>
   </si>
   <si>
@@ -344,13 +341,25 @@
   </si>
   <si>
     <t>Efetua pesquisa de utilizadores por nome e tag</t>
+  </si>
+  <si>
+    <t>Tagcloud criada em linha visto não haver bibliotecas para gerar imagens</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ViewBag.networkSize, falta um nivel está até ao segundo</t>
+  </si>
+  <si>
+    <t>Ficou a faltar o link para os leaderboards</t>
+  </si>
+  <si>
+    <t>Done!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,8 +388,15 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,6 +418,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -479,6 +501,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,9 +915,15 @@
       <c r="K6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="L6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -924,7 +961,7 @@
         <v>30</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>15</v>
@@ -953,18 +990,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="18" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -1046,7 +1083,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
@@ -1056,8 +1093,8 @@
       <c r="D11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>46</v>
+      <c r="E11" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>15</v>
@@ -1075,9 +1112,15 @@
       <c r="K11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+      <c r="L11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -1085,15 +1128,15 @@
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
@@ -1112,9 +1155,15 @@
       <c r="K12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
+      <c r="L12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
@@ -1140,8 +1189,12 @@
         <v>37</v>
       </c>
       <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="M13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
@@ -1149,7 +1202,7 @@
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="2:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1163,7 +1216,7 @@
       <c r="J14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="19" t="s">
         <v>38</v>
       </c>
       <c r="L14" s="8" t="s">
@@ -1190,10 +1243,10 @@
         <v>11</v>
       </c>
       <c r="J15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -1361,7 +1414,7 @@
     <mergeCell ref="J4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#56 Created Method and View to list frinds of user
</commit_message>
<xml_diff>
--- a/documentation/tasks/apoioMVC.xlsx
+++ b/documentation/tasks/apoioMVC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScarePT\Documents\EpicWare\documentation\tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Márcio\Dropbox\Faculdade\3º Ano\LAPR5\git\documentation\tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>Controller</t>
   </si>
@@ -301,13 +301,6 @@
     <t>Mostra a tag cloud das suas relações</t>
   </si>
   <si>
-    <t>Pagina que mostra todos os amigos do user autenticado</t>
-  </si>
-  <si>
-    <t>Acede diretamente ao user autenticado a partir da view
-para visualizar as connections do user</t>
-  </si>
-  <si>
     <t>NOVO</t>
   </si>
   <si>
@@ -353,6 +346,19 @@
   </si>
   <si>
     <t>Done!</t>
+  </si>
+  <si>
+    <t>Pagina que mostra todos os amigos do user</t>
+  </si>
+  <si>
+    <t>Recebe uma Lista de Users</t>
+  </si>
+  <si>
+    <t>FrindsList</t>
+  </si>
+  <si>
+    <t>Pesquisa todos os users amigos do user 
+id recebido por parametro</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -496,12 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -510,6 +510,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,21 +828,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="J4" s="16" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="J4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -916,7 +925,7 @@
         <v>13</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>15</v>
@@ -942,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>15</v>
@@ -961,7 +970,7 @@
         <v>30</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>15</v>
@@ -990,18 +999,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -1053,7 +1062,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>15</v>
@@ -1069,10 +1078,10 @@
         <v>34</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -1094,7 +1103,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>15</v>
@@ -1113,7 +1122,7 @@
         <v>35</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>15</v>
@@ -1133,10 +1142,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
@@ -1156,7 +1165,7 @@
         <v>36</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>15</v>
@@ -1171,13 +1180,23 @@
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+    <row r="13" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>55</v>
+      </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="H13" s="9"/>
       <c r="I13" s="10" t="s">
         <v>19</v>
@@ -1202,7 +1221,7 @@
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="2:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1216,14 +1235,18 @@
       <c r="J14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="19" t="s">
-        <v>38</v>
+      <c r="K14" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -1243,10 +1266,10 @@
         <v>11</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -1394,7 +1417,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -1405,7 +1428,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>